<commit_message>
problems with making connection to db to work and upd of tidsplan
</commit_message>
<xml_diff>
--- a/Tidsplan_xjobb.xlsx
+++ b/Tidsplan_xjobb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl.schlyter/OneDriveDentsu/localhost/examensarbete_a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B1E80B-2D90-6A4A-A653-413854CD12DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A572B3-5EA4-E64F-B464-199C43FFB2AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{283ADF86-6020-3D41-9AD4-19E14A7A3190}"/>
   </bookViews>
@@ -216,9 +216,6 @@
     <t>Also incl learning to work with git om a mac</t>
   </si>
   <si>
-    <t>2020-01-14 Pending</t>
-  </si>
-  <si>
     <t>Added necessairy tasks</t>
   </si>
   <si>
@@ -250,6 +247,9 @@
   </si>
   <si>
     <t>2020-01-29 Pending</t>
+  </si>
+  <si>
+    <t>2020-01-30 Pending</t>
   </si>
 </sst>
 </file>
@@ -647,9 +647,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1776197E-6351-F840-8D43-A3A4BE97CA17}">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q18" sqref="Q18"/>
+      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,7 +833,7 @@
         <v>11</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R11" t="s">
         <v>31</v>
@@ -942,17 +942,17 @@
         <v>36</v>
       </c>
       <c r="P15">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="Q15" s="6" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="S15">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="T15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="19" x14ac:dyDescent="0.25">
@@ -1014,7 +1014,7 @@
         <v>5</v>
       </c>
       <c r="Q18" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R18" t="s">
         <v>31</v>
@@ -1113,7 +1113,7 @@
         <v>3</v>
       </c>
       <c r="Q22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R22" t="s">
         <v>37</v>
@@ -1143,7 +1143,7 @@
         <v>9</v>
       </c>
       <c r="Q23" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R23" t="s">
         <v>33</v>
@@ -1153,7 +1153,7 @@
         <v>-1</v>
       </c>
       <c r="T23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="6:20" x14ac:dyDescent="0.2">
@@ -1386,11 +1386,11 @@
       </c>
       <c r="P36">
         <f>SUM(P10:P35)</f>
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="S36">
         <f>SUM(S10:S35)</f>
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="6:19" x14ac:dyDescent="0.2">
@@ -1406,11 +1406,11 @@
       </c>
       <c r="P37">
         <f>P36/8</f>
-        <v>7.25</v>
+        <v>7.625</v>
       </c>
       <c r="S37">
         <f>S36/8</f>
-        <v>4.25</v>
+        <v>3.875</v>
       </c>
     </row>
     <row r="38" spans="6:19" x14ac:dyDescent="0.2">
@@ -1419,17 +1419,17 @@
       </c>
       <c r="P38" s="7">
         <f>(P36/M36)*100</f>
-        <v>19.727891156462583</v>
+        <v>20.748299319727892</v>
       </c>
     </row>
     <row r="40" spans="6:19" ht="19" x14ac:dyDescent="0.25">
       <c r="F40" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="6:19" x14ac:dyDescent="0.2">
       <c r="F41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P41">
         <v>19</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="42" spans="6:19" x14ac:dyDescent="0.2">
       <c r="O42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P42">
         <f>SUM(P41)</f>
@@ -1452,11 +1452,11 @@
     </row>
     <row r="43" spans="6:19" x14ac:dyDescent="0.2">
       <c r="O43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P43">
         <f>P42+P36</f>
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="6:19" x14ac:dyDescent="0.2">
@@ -1465,16 +1465,16 @@
       </c>
       <c r="P44" s="9">
         <f>P43/8</f>
-        <v>9.625</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="6:19" x14ac:dyDescent="0.2">
       <c r="O45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P45" s="8">
         <f>P43/(M36+P42)</f>
-        <v>0.24600638977635783</v>
+        <v>0.25559105431309903</v>
       </c>
     </row>
     <row r="46" spans="6:19" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
remade initial api cause it is not working and upd of tidsplan
</commit_message>
<xml_diff>
--- a/Tidsplan_xjobb.xlsx
+++ b/Tidsplan_xjobb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl.schlyter/OneDriveDentsu/localhost/examensarbete_a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A572B3-5EA4-E64F-B464-199C43FFB2AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C71BD62-B7F3-554F-9253-4F31B2456763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{283ADF86-6020-3D41-9AD4-19E14A7A3190}"/>
   </bookViews>
@@ -647,9 +647,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1776197E-6351-F840-8D43-A3A4BE97CA17}">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomLeft" activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -942,14 +942,14 @@
         <v>36</v>
       </c>
       <c r="P15">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>71</v>
       </c>
       <c r="S15">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="T15" t="s">
         <v>62</v>
@@ -1386,11 +1386,11 @@
       </c>
       <c r="P36">
         <f>SUM(P10:P35)</f>
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="S36">
         <f>SUM(S10:S35)</f>
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="6:19" x14ac:dyDescent="0.2">
@@ -1406,11 +1406,11 @@
       </c>
       <c r="P37">
         <f>P36/8</f>
-        <v>7.625</v>
+        <v>8.125</v>
       </c>
       <c r="S37">
         <f>S36/8</f>
-        <v>3.875</v>
+        <v>3.375</v>
       </c>
     </row>
     <row r="38" spans="6:19" x14ac:dyDescent="0.2">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="P38" s="7">
         <f>(P36/M36)*100</f>
-        <v>20.748299319727892</v>
+        <v>22.108843537414966</v>
       </c>
     </row>
     <row r="40" spans="6:19" ht="19" x14ac:dyDescent="0.25">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="P43">
         <f>P42+P36</f>
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="6:19" x14ac:dyDescent="0.2">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="P44" s="9">
         <f>P43/8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="45" spans="6:19" x14ac:dyDescent="0.2">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="P45" s="8">
         <f>P43/(M36+P42)</f>
-        <v>0.25559105431309903</v>
+        <v>0.26837060702875398</v>
       </c>
     </row>
     <row r="46" spans="6:19" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
continued struggle  with making db connection to work
</commit_message>
<xml_diff>
--- a/Tidsplan_xjobb.xlsx
+++ b/Tidsplan_xjobb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl.schlyter/OneDriveDentsu/localhost/examensarbete_a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C71BD62-B7F3-554F-9253-4F31B2456763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8903B134-887E-594D-A9B7-1F976DD4D862}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{283ADF86-6020-3D41-9AD4-19E14A7A3190}"/>
   </bookViews>
@@ -222,9 +222,6 @@
     <t>Rekapitulera vanilla js</t>
   </si>
   <si>
-    <t>Plus a buch of off office hours, problem making connection to db work</t>
-  </si>
-  <si>
     <t>Sum added tasks</t>
   </si>
   <si>
@@ -249,7 +246,10 @@
     <t>2020-01-29 Pending</t>
   </si>
   <si>
-    <t>2020-01-30 Pending</t>
+    <t>2020-01-31 Pending</t>
+  </si>
+  <si>
+    <t>Plus a bunch of off office hours, problem making connection to db work</t>
   </si>
 </sst>
 </file>
@@ -647,9 +647,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1776197E-6351-F840-8D43-A3A4BE97CA17}">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q15" sqref="Q15"/>
+      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,7 +833,7 @@
         <v>11</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="R11" t="s">
         <v>31</v>
@@ -942,17 +942,17 @@
         <v>36</v>
       </c>
       <c r="P15">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S15">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="T15" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="19" x14ac:dyDescent="0.25">
@@ -1014,7 +1014,7 @@
         <v>5</v>
       </c>
       <c r="Q18" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R18" t="s">
         <v>31</v>
@@ -1113,7 +1113,7 @@
         <v>3</v>
       </c>
       <c r="Q22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="R22" t="s">
         <v>37</v>
@@ -1143,7 +1143,7 @@
         <v>9</v>
       </c>
       <c r="Q23" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R23" t="s">
         <v>33</v>
@@ -1153,7 +1153,7 @@
         <v>-1</v>
       </c>
       <c r="T23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="6:20" x14ac:dyDescent="0.2">
@@ -1386,11 +1386,11 @@
       </c>
       <c r="P36">
         <f>SUM(P10:P35)</f>
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="S36">
         <f>SUM(S10:S35)</f>
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="6:19" x14ac:dyDescent="0.2">
@@ -1406,11 +1406,11 @@
       </c>
       <c r="P37">
         <f>P36/8</f>
-        <v>8.125</v>
+        <v>8.5</v>
       </c>
       <c r="S37">
         <f>S36/8</f>
-        <v>3.375</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="6:19" x14ac:dyDescent="0.2">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="P38" s="7">
         <f>(P36/M36)*100</f>
-        <v>22.108843537414966</v>
+        <v>23.129251700680271</v>
       </c>
     </row>
     <row r="40" spans="6:19" ht="19" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
     </row>
     <row r="42" spans="6:19" x14ac:dyDescent="0.2">
       <c r="O42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P42">
         <f>SUM(P41)</f>
@@ -1452,11 +1452,11 @@
     </row>
     <row r="43" spans="6:19" x14ac:dyDescent="0.2">
       <c r="O43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P43">
         <f>P42+P36</f>
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="6:19" x14ac:dyDescent="0.2">
@@ -1465,16 +1465,16 @@
       </c>
       <c r="P44" s="9">
         <f>P43/8</f>
-        <v>10.5</v>
+        <v>10.875</v>
       </c>
     </row>
     <row r="45" spans="6:19" x14ac:dyDescent="0.2">
       <c r="O45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P45" s="8">
         <f>P43/(M36+P42)</f>
-        <v>0.26837060702875398</v>
+        <v>0.27795527156549521</v>
       </c>
     </row>
     <row r="46" spans="6:19" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
created test table in db with corresp read and craete models and apis
</commit_message>
<xml_diff>
--- a/Tidsplan_xjobb.xlsx
+++ b/Tidsplan_xjobb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl.schlyter/OneDriveDentsu/localhost/examensarbete_a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C721B6-7B89-7C49-A328-AD0068DB0BBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0842722F-A584-564E-9202-75BE7AE3850A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{283ADF86-6020-3D41-9AD4-19E14A7A3190}"/>
   </bookViews>
@@ -249,7 +249,7 @@
     <t>2020-02-06 Pending</t>
   </si>
   <si>
-    <t>Plus a bunch of off office hours, problem making connection to db work due to blank space in sql syntax, but generally underestimated</t>
+    <t>Plus a bunch of off office hours, problem making connection to db due to blank space in sql syntax, but generally underestimated</t>
   </si>
 </sst>
 </file>
@@ -647,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1776197E-6351-F840-8D43-A3A4BE97CA17}">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added test page for work with making post connection to work for app
</commit_message>
<xml_diff>
--- a/Tidsplan_xjobb.xlsx
+++ b/Tidsplan_xjobb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl.schlyter/OneDriveDentsu/localhost/examensarbete_a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C058112-2BAC-DB41-93FE-4BAA9B3525BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD838D8E-A1DC-0847-9243-B41E6F7114D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{283ADF86-6020-3D41-9AD4-19E14A7A3190}"/>
   </bookViews>
@@ -251,10 +251,10 @@
     <t>Plus a bunch of off office hours, problem making connection to db due to blank space in sql syntax, but generally underestimated</t>
   </si>
   <si>
-    <t>2020-02-11 Pending</t>
-  </si>
-  <si>
     <t>Greate trouble making it work to update db via react app</t>
+  </si>
+  <si>
+    <t>2020-02-14 Pending</t>
   </si>
 </sst>
 </file>
@@ -653,8 +653,8 @@
   <dimension ref="A1:T46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q19" sqref="Q19"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1052,20 +1052,20 @@
         <v>31</v>
       </c>
       <c r="P19">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Q19" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="R19" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="S19">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="T19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="6:20" x14ac:dyDescent="0.2">
@@ -1409,11 +1409,11 @@
       </c>
       <c r="P36">
         <f>SUM(P10:P35)</f>
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="S36">
         <f>SUM(S10:S35)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="6:19" x14ac:dyDescent="0.2">
@@ -1429,11 +1429,11 @@
       </c>
       <c r="P37">
         <f>P36/8</f>
-        <v>11.25</v>
+        <v>11.625</v>
       </c>
       <c r="S37">
         <f>S36/8</f>
-        <v>1.25</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="38" spans="6:19" x14ac:dyDescent="0.2">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="P38" s="7">
         <f>(P36/M36)*100</f>
-        <v>30.612244897959183</v>
+        <v>31.632653061224492</v>
       </c>
     </row>
     <row r="40" spans="6:19" ht="19" x14ac:dyDescent="0.25">
@@ -1479,7 +1479,7 @@
       </c>
       <c r="P43">
         <f>P42+P36</f>
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="6:19" x14ac:dyDescent="0.2">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="P44" s="9">
         <f>P43/8</f>
-        <v>13.625</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="6:19" x14ac:dyDescent="0.2">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P45" s="8">
         <f>P43/(M36+P42)</f>
-        <v>0.34824281150159747</v>
+        <v>0.35782747603833864</v>
       </c>
     </row>
     <row r="46" spans="6:19" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
cont work with making post to work from app
</commit_message>
<xml_diff>
--- a/Tidsplan_xjobb.xlsx
+++ b/Tidsplan_xjobb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl.schlyter/OneDriveDentsu/localhost/examensarbete_a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD838D8E-A1DC-0847-9243-B41E6F7114D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D554F9DF-DC1F-8248-B092-1A49300568AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{283ADF86-6020-3D41-9AD4-19E14A7A3190}"/>
   </bookViews>
@@ -254,7 +254,7 @@
     <t>Greate trouble making it work to update db via react app</t>
   </si>
   <si>
-    <t>2020-02-14 Pending</t>
+    <t>2020-02-17 Pending</t>
   </si>
 </sst>
 </file>
@@ -1052,17 +1052,17 @@
         <v>31</v>
       </c>
       <c r="P19">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>73</v>
       </c>
       <c r="R19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S19">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="T19" t="s">
         <v>72</v>
@@ -1409,11 +1409,11 @@
       </c>
       <c r="P36">
         <f>SUM(P10:P35)</f>
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="S36">
         <f>SUM(S10:S35)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="6:19" x14ac:dyDescent="0.2">
@@ -1429,11 +1429,11 @@
       </c>
       <c r="P37">
         <f>P36/8</f>
-        <v>11.625</v>
+        <v>12</v>
       </c>
       <c r="S37">
         <f>S36/8</f>
-        <v>0.875</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="38" spans="6:19" x14ac:dyDescent="0.2">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="P38" s="7">
         <f>(P36/M36)*100</f>
-        <v>31.632653061224492</v>
+        <v>32.653061224489797</v>
       </c>
     </row>
     <row r="40" spans="6:19" ht="19" x14ac:dyDescent="0.25">
@@ -1479,7 +1479,7 @@
       </c>
       <c r="P43">
         <f>P42+P36</f>
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="6:19" x14ac:dyDescent="0.2">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="P44" s="9">
         <f>P43/8</f>
-        <v>14</v>
+        <v>14.375</v>
       </c>
     </row>
     <row r="45" spans="6:19" x14ac:dyDescent="0.2">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P45" s="8">
         <f>P43/(M36+P42)</f>
-        <v>0.35782747603833864</v>
+        <v>0.36741214057507987</v>
       </c>
     </row>
     <row r="46" spans="6:19" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Solved main  post to db issue for now
</commit_message>
<xml_diff>
--- a/Tidsplan_xjobb.xlsx
+++ b/Tidsplan_xjobb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl.schlyter/OneDriveDentsu/localhost/examensarbete_a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D829C65-83C5-DC45-95A4-33EB640A1FD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA86BA7B-E6D1-F147-89E2-594C2ECC9471}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{283ADF86-6020-3D41-9AD4-19E14A7A3190}"/>
   </bookViews>
@@ -251,10 +251,10 @@
     <t>Plus a bunch of off office hours, problem making connection to db due to blank space in sql syntax, but generally underestimated</t>
   </si>
   <si>
-    <t>Greate trouble making it work to update db via react app</t>
-  </si>
-  <si>
-    <t>2020-02-27 Pending</t>
+    <t>2020-02-28 Pending</t>
+  </si>
+  <si>
+    <t>Greate trouble making it work to update db via react app. Finally got through..</t>
   </si>
 </sst>
 </file>
@@ -652,9 +652,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1776197E-6351-F840-8D43-A3A4BE97CA17}">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1052,20 +1052,20 @@
         <v>31</v>
       </c>
       <c r="P19">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="Q19" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R19" t="s">
         <v>35</v>
       </c>
       <c r="S19">
         <f t="shared" si="1"/>
-        <v>-17</v>
+        <v>-24</v>
       </c>
       <c r="T19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="6:20" x14ac:dyDescent="0.2">
@@ -1409,11 +1409,11 @@
       </c>
       <c r="P36">
         <f>SUM(P10:P35)</f>
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="S36">
         <f>SUM(S10:S35)</f>
-        <v>-9</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="37" spans="6:19" x14ac:dyDescent="0.2">
@@ -1429,11 +1429,11 @@
       </c>
       <c r="P37">
         <f>P36/8</f>
-        <v>13.625</v>
+        <v>14.5</v>
       </c>
       <c r="S37">
         <f>S36/8</f>
-        <v>-1.125</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="38" spans="6:19" x14ac:dyDescent="0.2">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="P38" s="7">
         <f>(P36/M36)*100</f>
-        <v>37.074829931972793</v>
+        <v>39.455782312925166</v>
       </c>
     </row>
     <row r="40" spans="6:19" ht="19" x14ac:dyDescent="0.25">
@@ -1479,7 +1479,7 @@
       </c>
       <c r="P43">
         <f>P42+P36</f>
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="6:19" x14ac:dyDescent="0.2">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="P44" s="9">
         <f>P43/8</f>
-        <v>16</v>
+        <v>16.875</v>
       </c>
     </row>
     <row r="45" spans="6:19" x14ac:dyDescent="0.2">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P45" s="8">
         <f>P43/(M36+P42)</f>
-        <v>0.40894568690095845</v>
+        <v>0.43130990415335463</v>
       </c>
     </row>
     <row r="46" spans="6:19" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Mainly added user authentication endpoint
</commit_message>
<xml_diff>
--- a/Tidsplan_xjobb.xlsx
+++ b/Tidsplan_xjobb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl.schlyter/OneDriveDentsu/localhost/examensarbete_a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA86BA7B-E6D1-F147-89E2-594C2ECC9471}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4879EF02-4B29-1E4B-8C89-61889B36FEE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{283ADF86-6020-3D41-9AD4-19E14A7A3190}"/>
   </bookViews>
@@ -251,10 +251,10 @@
     <t>Plus a bunch of off office hours, problem making connection to db due to blank space in sql syntax, but generally underestimated</t>
   </si>
   <si>
-    <t>2020-02-28 Pending</t>
-  </si>
-  <si>
     <t>Greate trouble making it work to update db via react app. Finally got through..</t>
+  </si>
+  <si>
+    <t>2020-03-03 Pending</t>
   </si>
 </sst>
 </file>
@@ -1052,20 +1052,20 @@
         <v>31</v>
       </c>
       <c r="P19">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="Q19" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="R19" t="s">
         <v>35</v>
       </c>
       <c r="S19">
         <f t="shared" si="1"/>
-        <v>-24</v>
+        <v>-35</v>
       </c>
       <c r="T19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="6:20" x14ac:dyDescent="0.2">
@@ -1409,11 +1409,11 @@
       </c>
       <c r="P36">
         <f>SUM(P10:P35)</f>
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="S36">
         <f>SUM(S10:S35)</f>
-        <v>-16</v>
+        <v>-27</v>
       </c>
     </row>
     <row r="37" spans="6:19" x14ac:dyDescent="0.2">
@@ -1429,11 +1429,11 @@
       </c>
       <c r="P37">
         <f>P36/8</f>
-        <v>14.5</v>
+        <v>15.875</v>
       </c>
       <c r="S37">
         <f>S36/8</f>
-        <v>-2</v>
+        <v>-3.375</v>
       </c>
     </row>
     <row r="38" spans="6:19" x14ac:dyDescent="0.2">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="P38" s="7">
         <f>(P36/M36)*100</f>
-        <v>39.455782312925166</v>
+        <v>43.197278911564624</v>
       </c>
     </row>
     <row r="40" spans="6:19" ht="19" x14ac:dyDescent="0.25">
@@ -1479,7 +1479,7 @@
       </c>
       <c r="P43">
         <f>P42+P36</f>
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="6:19" x14ac:dyDescent="0.2">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="P44" s="9">
         <f>P43/8</f>
-        <v>16.875</v>
+        <v>18.25</v>
       </c>
     </row>
     <row r="45" spans="6:19" x14ac:dyDescent="0.2">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P45" s="8">
         <f>P43/(M36+P42)</f>
-        <v>0.43130990415335463</v>
+        <v>0.46645367412140576</v>
       </c>
     </row>
     <row r="46" spans="6:19" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added toplist endpoint to api
</commit_message>
<xml_diff>
--- a/Tidsplan_xjobb.xlsx
+++ b/Tidsplan_xjobb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl.schlyter/OneDriveDentsu/localhost/examensarbete_a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4879EF02-4B29-1E4B-8C89-61889B36FEE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5038A955-A454-E541-A03D-F26FCDD94F52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{283ADF86-6020-3D41-9AD4-19E14A7A3190}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
   <si>
     <t>Features</t>
   </si>
@@ -251,10 +251,13 @@
     <t>Plus a bunch of off office hours, problem making connection to db due to blank space in sql syntax, but generally underestimated</t>
   </si>
   <si>
-    <t>Greate trouble making it work to update db via react app. Finally got through..</t>
-  </si>
-  <si>
-    <t>2020-03-03 Pending</t>
+    <t>2020-03-12 Pending</t>
+  </si>
+  <si>
+    <t>Greate trouble making it work to update db via react app. Then great trouble sending all user fields to db. Finally got through with support from Rakib</t>
+  </si>
+  <si>
+    <t>2020-03-23 Pending</t>
   </si>
 </sst>
 </file>
@@ -652,9 +655,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1776197E-6351-F840-8D43-A3A4BE97CA17}">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1028,7 +1031,7 @@
         <v>31</v>
       </c>
       <c r="S18">
-        <f t="shared" ref="S18:S19" si="1">M18-P18</f>
+        <f t="shared" ref="S18:S21" si="1">M18-P18</f>
         <v>-1</v>
       </c>
     </row>
@@ -1052,20 +1055,20 @@
         <v>31</v>
       </c>
       <c r="P19">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="Q19" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R19" t="s">
         <v>35</v>
       </c>
       <c r="S19">
         <f t="shared" si="1"/>
-        <v>-35</v>
+        <v>-55</v>
       </c>
       <c r="T19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="6:20" x14ac:dyDescent="0.2">
@@ -1090,7 +1093,19 @@
       <c r="O20" t="s">
         <v>33</v>
       </c>
-      <c r="Q20" s="6"/>
+      <c r="P20">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>43902</v>
+      </c>
+      <c r="R20" t="s">
+        <v>36</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="6:20" x14ac:dyDescent="0.2">
       <c r="G21" t="s">
@@ -1111,7 +1126,19 @@
       <c r="O21" t="s">
         <v>35</v>
       </c>
-      <c r="Q21" s="6"/>
+      <c r="P21">
+        <v>28</v>
+      </c>
+      <c r="Q21" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="R21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="1"/>
+        <v>-20</v>
+      </c>
     </row>
     <row r="22" spans="6:20" x14ac:dyDescent="0.2">
       <c r="F22" t="s">
@@ -1291,6 +1318,15 @@
         <v>43865</v>
       </c>
       <c r="O29" t="s">
+        <v>31</v>
+      </c>
+      <c r="P29">
+        <v>8</v>
+      </c>
+      <c r="Q29" s="6">
+        <v>43921</v>
+      </c>
+      <c r="R29" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1409,11 +1445,11 @@
       </c>
       <c r="P36">
         <f>SUM(P10:P35)</f>
-        <v>127</v>
+        <v>186</v>
       </c>
       <c r="S36">
         <f>SUM(S10:S35)</f>
-        <v>-27</v>
+        <v>-66</v>
       </c>
     </row>
     <row r="37" spans="6:19" x14ac:dyDescent="0.2">
@@ -1429,11 +1465,11 @@
       </c>
       <c r="P37">
         <f>P36/8</f>
-        <v>15.875</v>
+        <v>23.25</v>
       </c>
       <c r="S37">
         <f>S36/8</f>
-        <v>-3.375</v>
+        <v>-8.25</v>
       </c>
     </row>
     <row r="38" spans="6:19" x14ac:dyDescent="0.2">
@@ -1442,7 +1478,7 @@
       </c>
       <c r="P38" s="7">
         <f>(P36/M36)*100</f>
-        <v>43.197278911564624</v>
+        <v>63.265306122448983</v>
       </c>
     </row>
     <row r="40" spans="6:19" ht="19" x14ac:dyDescent="0.25">
@@ -1479,7 +1515,7 @@
       </c>
       <c r="P43">
         <f>P42+P36</f>
-        <v>146</v>
+        <v>205</v>
       </c>
     </row>
     <row r="44" spans="6:19" x14ac:dyDescent="0.2">
@@ -1488,7 +1524,7 @@
       </c>
       <c r="P44" s="9">
         <f>P43/8</f>
-        <v>18.25</v>
+        <v>25.625</v>
       </c>
     </row>
     <row r="45" spans="6:19" x14ac:dyDescent="0.2">
@@ -1497,7 +1533,7 @@
       </c>
       <c r="P45" s="8">
         <f>P43/(M36+P42)</f>
-        <v>0.46645367412140576</v>
+        <v>0.65495207667731625</v>
       </c>
     </row>
     <row r="46" spans="6:19" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Testing create bet api with hardcoded pieces
</commit_message>
<xml_diff>
--- a/Tidsplan_xjobb.xlsx
+++ b/Tidsplan_xjobb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl.schlyter/OneDriveDentsu/localhost/examensarbete_a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5038A955-A454-E541-A03D-F26FCDD94F52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33D571E-0416-3F46-ACDE-38B074E2073A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{283ADF86-6020-3D41-9AD4-19E14A7A3190}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
   <si>
     <t>Features</t>
   </si>
@@ -258,6 +258,12 @@
   </si>
   <si>
     <t>2020-03-23 Pending</t>
+  </si>
+  <si>
+    <t>2020-04-03 Pending</t>
+  </si>
+  <si>
+    <t>Guessers Average Component</t>
   </si>
 </sst>
 </file>
@@ -653,11 +659,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1776197E-6351-F840-8D43-A3A4BE97CA17}">
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1243,7 +1249,19 @@
       <c r="O25" t="s">
         <v>33</v>
       </c>
-      <c r="Q25" s="6"/>
+      <c r="P25">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="6">
+        <v>43922</v>
+      </c>
+      <c r="R25" t="s">
+        <v>33</v>
+      </c>
+      <c r="S25">
+        <f>M25-P25</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="6:20" x14ac:dyDescent="0.2">
       <c r="G26" t="s">
@@ -1261,7 +1279,19 @@
       <c r="O26" t="s">
         <v>35</v>
       </c>
-      <c r="Q26" s="6"/>
+      <c r="P26">
+        <v>10</v>
+      </c>
+      <c r="Q26" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="R26" t="s">
+        <v>36</v>
+      </c>
+      <c r="S26">
+        <f>M26-P26</f>
+        <v>-2</v>
+      </c>
     </row>
     <row r="27" spans="6:20" x14ac:dyDescent="0.2">
       <c r="G27" t="s">
@@ -1328,6 +1358,10 @@
       </c>
       <c r="R29" t="s">
         <v>31</v>
+      </c>
+      <c r="S29">
+        <f>M29-P29</f>
+        <v>-2</v>
       </c>
     </row>
     <row r="30" spans="6:20" x14ac:dyDescent="0.2">
@@ -1445,11 +1479,11 @@
       </c>
       <c r="P36">
         <f>SUM(P10:P35)</f>
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="S36">
         <f>SUM(S10:S35)</f>
-        <v>-66</v>
+        <v>-70</v>
       </c>
     </row>
     <row r="37" spans="6:19" x14ac:dyDescent="0.2">
@@ -1457,19 +1491,19 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <f>M36/8</f>
-        <v>36.75</v>
+        <f>M36/7</f>
+        <v>42</v>
       </c>
       <c r="O37" t="s">
         <v>28</v>
       </c>
-      <c r="P37">
-        <f>P36/8</f>
-        <v>23.25</v>
+      <c r="P37" s="7">
+        <f>P36/7</f>
+        <v>28.571428571428573</v>
       </c>
       <c r="S37">
         <f>S36/8</f>
-        <v>-8.25</v>
+        <v>-8.75</v>
       </c>
     </row>
     <row r="38" spans="6:19" x14ac:dyDescent="0.2">
@@ -1478,7 +1512,7 @@
       </c>
       <c r="P38" s="7">
         <f>(P36/M36)*100</f>
-        <v>63.265306122448983</v>
+        <v>68.027210884353735</v>
       </c>
     </row>
     <row r="40" spans="6:19" ht="19" x14ac:dyDescent="0.25">
@@ -1501,43 +1535,57 @@
       </c>
     </row>
     <row r="42" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="O42" t="s">
-        <v>62</v>
+      <c r="F42" t="s">
+        <v>76</v>
       </c>
       <c r="P42">
-        <f>SUM(P41)</f>
-        <v>19</v>
+        <v>4</v>
+      </c>
+      <c r="Q42" s="6">
+        <v>43923</v>
+      </c>
+      <c r="R42" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="6:19" x14ac:dyDescent="0.2">
       <c r="O43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P43">
-        <f>P42+P36</f>
-        <v>205</v>
+        <f>SUM(P41:P42)</f>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="6:19" x14ac:dyDescent="0.2">
       <c r="O44" t="s">
-        <v>28</v>
-      </c>
-      <c r="P44" s="9">
-        <f>P43/8</f>
-        <v>25.625</v>
+        <v>63</v>
+      </c>
+      <c r="P44">
+        <f>P43+P36</f>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="6:19" x14ac:dyDescent="0.2">
       <c r="O45" t="s">
+        <v>28</v>
+      </c>
+      <c r="P45" s="9">
+        <f>P44/7</f>
+        <v>31.857142857142858</v>
+      </c>
+    </row>
+    <row r="46" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="O46" t="s">
         <v>66</v>
       </c>
-      <c r="P45" s="8">
-        <f>P43/(M36+P42)</f>
-        <v>0.65495207667731625</v>
-      </c>
-    </row>
-    <row r="46" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="P46" s="8"/>
+      <c r="P46" s="8">
+        <f>P44/(M36+P43)</f>
+        <v>0.70347003154574128</v>
+      </c>
+    </row>
+    <row r="47" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="P47" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>